<commit_message>
Legende etwas erweitert, aber noch nicht vollständig
</commit_message>
<xml_diff>
--- a/Berechnungen/Legende.xlsx
+++ b/Berechnungen/Legende.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marvi\Desktop\Maschinenelemente 3\Entwurf\Gruppe 9\Gruppe9_ME3E\Berechnungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA9D997-FB1D-4169-A4F7-BB4AE175F523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75810EB4-5A04-47DD-8870-EE0A75404EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14715" yWindow="1770" windowWidth="21600" windowHeight="11385" xr2:uid="{461ED94B-406C-4008-BC61-809AC2BF0740}"/>
+    <workbookView xWindow="5400" yWindow="1365" windowWidth="21600" windowHeight="11385" xr2:uid="{461ED94B-406C-4008-BC61-809AC2BF0740}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="213">
   <si>
     <t>Abkürzung</t>
   </si>
@@ -1592,13 +1592,288 @@
   </si>
   <si>
     <t>Dauerfestigkeitsschubspannung von 42CrMo4</t>
+  </si>
+  <si>
+    <t>Rm</t>
+  </si>
+  <si>
+    <t>Rp0;2N</t>
+  </si>
+  <si>
+    <t>σbWN</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12.65"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>tWN</t>
+    </r>
+  </si>
+  <si>
+    <t>Rz</t>
+  </si>
+  <si>
+    <t>Dehngrenze</t>
+  </si>
+  <si>
+    <t>Zugfestigkeit</t>
+  </si>
+  <si>
+    <t>Rautiefe</t>
+  </si>
+  <si>
+    <t>X1 - X7</t>
+  </si>
+  <si>
+    <t>Längen der Wellenabschnitte</t>
+  </si>
+  <si>
+    <t>FBy1 - FBy3</t>
+  </si>
+  <si>
+    <t>FAy1 - FAy3</t>
+  </si>
+  <si>
+    <t>FAz1 - FAz3</t>
+  </si>
+  <si>
+    <t>FBz1 - FBz3</t>
+  </si>
+  <si>
+    <t>FRA1 - FRA3</t>
+  </si>
+  <si>
+    <t>FRB1 - FRB3</t>
+  </si>
+  <si>
+    <t>Resultierende Lagerkraft im Lager A Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Resultierende Lagerkraft im Lager B Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>FAx1 - FAx3</t>
+  </si>
+  <si>
+    <t>Radiale Lagerkraft B XY-Ebene Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Radiale Lagerkraft A XY-Ebene Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Radiale Lagerkraft A XZ-Ebene Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Radiale Lagerkraft B XZ-Ebene Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Axiale Lagerkraft A XY/XZ-Ebene Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Axiale Lagerkraft B XY/XZ-Ebene Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>FBx1 - FBx3</t>
+  </si>
+  <si>
+    <t>s1min - s7min</t>
+  </si>
+  <si>
+    <t>Minimale Länge Strecke s1 bis s7</t>
+  </si>
+  <si>
+    <t>Maximale Länge Strecke s1 bis s7</t>
+  </si>
+  <si>
+    <t>s1max - s7max</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>FQ</t>
+  </si>
+  <si>
+    <t>Normalkraft</t>
+  </si>
+  <si>
+    <t>Querkraft</t>
+  </si>
+  <si>
+    <t>Ms1xy - Ms7xy</t>
+  </si>
+  <si>
+    <t>Moment um s1 bis s7 in XY-Ebene</t>
+  </si>
+  <si>
+    <t>Ms1xymin - Ms7xymin</t>
+  </si>
+  <si>
+    <t>Minimales Moment um s1 bis s7 in XY-Ebene</t>
+  </si>
+  <si>
+    <t>Ms1xymax - Ms7xymax</t>
+  </si>
+  <si>
+    <t>Maximales Moment um s1 bis s7 in XY-Ebene</t>
+  </si>
+  <si>
+    <t>s1 - s7</t>
+  </si>
+  <si>
+    <t>Strecken s1 bis s7 für Schnittgrößenverläufe</t>
+  </si>
+  <si>
+    <t>Ms1xz - Ms7xz</t>
+  </si>
+  <si>
+    <t>Moment um s1 bis s7 in XZ-Ebene</t>
+  </si>
+  <si>
+    <t>Ms1xzmax - Ms7xzmax</t>
+  </si>
+  <si>
+    <t>Ms1xzmin - Ms7xzmin</t>
+  </si>
+  <si>
+    <t>Minimales Moment um s1 bis s7 in XZ-Ebene</t>
+  </si>
+  <si>
+    <t>Maximales Moment um s1 bis s7 in XZ-Ebene</t>
+  </si>
+  <si>
+    <t>MsAmax</t>
+  </si>
+  <si>
+    <t>Maximales Drehmoment Antriebswelle</t>
+  </si>
+  <si>
+    <t>Maximales Drehmoment Abtriebswelle</t>
+  </si>
+  <si>
+    <t>Maximales Drehmoment Vorgelegewelle</t>
+  </si>
+  <si>
+    <t>MsVmax</t>
+  </si>
+  <si>
+    <t>MsWmax</t>
+  </si>
+  <si>
+    <t>Biegespannung</t>
+  </si>
+  <si>
+    <t>Torsionsspannung</t>
+  </si>
+  <si>
+    <t>WB1 - WB3</t>
+  </si>
+  <si>
+    <t>WT1 - WB3</t>
+  </si>
+  <si>
+    <t>Biegewiderstandsmoment Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Torsionswiderstandsmoment Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>σbmax1 - σbmax3</t>
+  </si>
+  <si>
+    <t>τtmax1 - τtmax3</t>
+  </si>
+  <si>
+    <t>Kt1 - Kt3</t>
+  </si>
+  <si>
+    <t>Technologischer Größeneinflussfaktor</t>
+  </si>
+  <si>
+    <t>σbF1 - σbF3</t>
+  </si>
+  <si>
+    <t>τtF1 - τtF3</t>
+  </si>
+  <si>
+    <t>SF1 - SF3</t>
+  </si>
+  <si>
+    <t>Sicherheit Fließgrenze Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>SF1min - SF3min</t>
+  </si>
+  <si>
+    <t>Mindestsicherheit Fließgrenze Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>σba1 - σba3</t>
+  </si>
+  <si>
+    <t>Maximale statische Biegespannung Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Maximale statische Torsionsspannung Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Statische Bauteilfestigkeit gegen Biegung Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Statische Bauteilfestigkeit gegen Torsion Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Dynamische Biegespannung Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>σbm1 - σbm3</t>
+  </si>
+  <si>
+    <t>Vernachlässigter Faktor dynamische Biegespannung</t>
+  </si>
+  <si>
+    <t>τta1 - τta3</t>
+  </si>
+  <si>
+    <t>τtm1 - τtm3</t>
+  </si>
+  <si>
+    <t>Dynamische Torsionsspannung Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Vernachlässigter Faktor dynamische Torsionsspannung</t>
+  </si>
+  <si>
+    <t>βkb1 - βkb3</t>
+  </si>
+  <si>
+    <t>Kerbwirkungszahl Biegung Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>βkt1 - βkt3</t>
+  </si>
+  <si>
+    <t>Kerbwirkungszahl Torsion Welle 1 bis 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1635,6 +1910,18 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12.65"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1644,7 +1931,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1710,17 +1997,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2035,15 +2334,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4572409-E229-4D26-A0D4-41F629C29121}">
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="50.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2560,31 +2859,352 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
+      <c r="A65" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
+      <c r="A66" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
+      <c r="A67" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
+      <c r="A69" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B69" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
+      <c r="A70" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B70" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B71" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B72" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B73" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B74" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B75" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B76" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B77" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B78" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B79" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B80" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B81" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B82" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B83" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B84" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B85" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B86" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B87" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B88" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B89" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B90" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B91" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B92" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B93" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B94" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B95" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B96" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B97" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B98" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B99" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B100" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B101" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B102" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B103" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B104" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B105" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B106" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B107" t="s">
+        <v>212</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Testat 1 vorbereitet, Legende MEINERSEITS aktualisiert
</commit_message>
<xml_diff>
--- a/Berechnungen/Legende.xlsx
+++ b/Berechnungen/Legende.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edisd\Documents\GitHub\Gruppe9_ME3E\Berechnungen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marvi\Desktop\Maschinenelemente 3\Entwurf\Gruppe 9\Gruppe9_ME3E\Berechnungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEFBCF9-6165-4FCC-8636-DC8A35EA5A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730D2369-C648-4D38-91F9-C127CDCFDF88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{461ED94B-406C-4008-BC61-809AC2BF0740}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{461ED94B-406C-4008-BC61-809AC2BF0740}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="246">
   <si>
     <t>Abkürzung</t>
   </si>
@@ -1594,26 +1594,1825 @@
     <t>Dauerfestigkeitsschubspannung von 42CrMo4</t>
   </si>
   <si>
-    <t>Rm</t>
-  </si>
-  <si>
-    <t>Rp0;2N</t>
-  </si>
-  <si>
-    <t>σbWN</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
+    <t>Rz</t>
+  </si>
+  <si>
+    <t>Dehngrenze</t>
+  </si>
+  <si>
+    <t>Zugfestigkeit</t>
+  </si>
+  <si>
+    <t>Rautiefe</t>
+  </si>
+  <si>
+    <t>Längen der Wellenabschnitte</t>
+  </si>
+  <si>
+    <t>Resultierende Lagerkraft im Lager A Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Resultierende Lagerkraft im Lager B Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Radiale Lagerkraft B XY-Ebene Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Radiale Lagerkraft A XY-Ebene Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Radiale Lagerkraft A XZ-Ebene Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Radiale Lagerkraft B XZ-Ebene Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Axiale Lagerkraft A XY/XZ-Ebene Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Axiale Lagerkraft B XY/XZ-Ebene Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Minimale Länge Strecke s1 bis s7</t>
+  </si>
+  <si>
+    <t>Maximale Länge Strecke s1 bis s7</t>
+  </si>
+  <si>
+    <t>Normalkraft</t>
+  </si>
+  <si>
+    <t>Querkraft</t>
+  </si>
+  <si>
+    <t>Moment um s1 bis s7 in XY-Ebene</t>
+  </si>
+  <si>
+    <t>Minimales Moment um s1 bis s7 in XY-Ebene</t>
+  </si>
+  <si>
+    <t>Maximales Moment um s1 bis s7 in XY-Ebene</t>
+  </si>
+  <si>
+    <t>Strecken s1 bis s7 für Schnittgrößenverläufe</t>
+  </si>
+  <si>
+    <t>Moment um s1 bis s7 in XZ-Ebene</t>
+  </si>
+  <si>
+    <t>Minimales Moment um s1 bis s7 in XZ-Ebene</t>
+  </si>
+  <si>
+    <t>Maximales Moment um s1 bis s7 in XZ-Ebene</t>
+  </si>
+  <si>
+    <t>Maximales Drehmoment Antriebswelle</t>
+  </si>
+  <si>
+    <t>Maximales Drehmoment Abtriebswelle</t>
+  </si>
+  <si>
+    <t>Maximales Drehmoment Vorgelegewelle</t>
+  </si>
+  <si>
+    <t>Biegespannung</t>
+  </si>
+  <si>
+    <t>Torsionsspannung</t>
+  </si>
+  <si>
+    <t>Biegewiderstandsmoment Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Torsionswiderstandsmoment Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Technologischer Größeneinflussfaktor</t>
+  </si>
+  <si>
+    <t>Sicherheit Fließgrenze Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Mindestsicherheit Fließgrenze Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Maximale statische Biegespannung Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Maximale statische Torsionsspannung Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Statische Bauteilfestigkeit gegen Biegung Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Statische Bauteilfestigkeit gegen Torsion Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Dynamische Biegespannung Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Vernachlässigter Faktor dynamische Biegespannung</t>
+  </si>
+  <si>
+    <t>Dynamische Torsionsspannung Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Vernachlässigter Faktor dynamische Torsionsspannung</t>
+  </si>
+  <si>
+    <t>Kerbwirkungszahl Biegung Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Kerbwirkungszahl Torsion Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>P1L</t>
+  </si>
+  <si>
+    <t>P1F</t>
+  </si>
+  <si>
+    <t>dynamische Lagerbelastung (Loslager - Antriebswelle)</t>
+  </si>
+  <si>
+    <t>dynamische Lagerbelastung (Festlager - Antriebswelle)</t>
+  </si>
+  <si>
+    <t>l10h</t>
+  </si>
+  <si>
+    <t>anzustrebende nominelle Lebensauer</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Lebensdauerexponent</t>
+  </si>
+  <si>
+    <t>Cerf</t>
+  </si>
+  <si>
+    <t>erforderliche dynamische Tragzahl</t>
+  </si>
+  <si>
+    <t>Geometrischer Größeneinflussfaktor</t>
+  </si>
+  <si>
+    <t>Oberflächen- Einflussfaktor Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Oberflächenverfestigungs- Einflussfaktor Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Konstruktionsfaktor Biegung Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Konstruktionsfaktor Torsion Welle 1 bis 3</t>
+  </si>
+  <si>
+    <t>Biege- Wechselfestigkeit</t>
+  </si>
+  <si>
+    <t>Torsions- Wechselfestigkeit</t>
+  </si>
+  <si>
+    <t>Mindestsicherheit Dauerfestigkeit</t>
+  </si>
+  <si>
+    <t>Dynamischer Sicherheitsfaktor</t>
+  </si>
+  <si>
+    <t>Erforderliche Dauerfestigkeit</t>
+  </si>
+  <si>
+    <t>Dynamische Gesamtsicherheit / Dauerfestigkeit</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>m</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p0;2N</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>By1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>By3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ay1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ay3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Az1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Az3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bz1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bz3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">RA1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>RA3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>RB1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>RB3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ax1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ax3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bx1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bx3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1min</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - s</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>7min</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1max</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - s</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>7max</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>N</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Q</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>s1xy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>s7xy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>s1xymin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>s7xymin</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>s1xymax</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>s7xymax</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - s</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>s1xz</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>s7xz</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>s1xzmin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>s7xzmin</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>s1xzmax</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>s7xzmax</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>sAmax</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>sVmax</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>sWmax</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>B1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - W</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>B3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>T1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - W</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>T3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>σ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>bmax1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - σ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>bmax3</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>τ</t>
     </r>
     <r>
       <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>tmax1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>tmax3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>t1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>t3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>σ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>bF1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - σ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>bF3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>tF1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>tF3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>F1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - S</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>F3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>F1min</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - S</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>F3min</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>σ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ba1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - σ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ba3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>σ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>bm1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - σ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>bm3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ta1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ta3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>tm1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>tm3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>β</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>kb1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - β</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>kb3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>β</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>kt1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - β</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>kt3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>g1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>g3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>0σ1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>0σ3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>0τ1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>0τ3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>V1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>V3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Db1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Db3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Dt1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Dt3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>σ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>bGW1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - σ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>bGW3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>D1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - S</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>D3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>D1min</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - S</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>D3min</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>z1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - S</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>z3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Derf1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - S</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Derf3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>σ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>bWN</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
         <sz val="12.65"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -1623,280 +3422,38 @@
     </r>
   </si>
   <si>
-    <t>Rz</t>
-  </si>
-  <si>
-    <t>Dehngrenze</t>
-  </si>
-  <si>
-    <t>Zugfestigkeit</t>
-  </si>
-  <si>
-    <t>Rautiefe</t>
-  </si>
-  <si>
-    <t>X1 - X7</t>
-  </si>
-  <si>
-    <t>Längen der Wellenabschnitte</t>
-  </si>
-  <si>
-    <t>FBy1 - FBy3</t>
-  </si>
-  <si>
-    <t>FAy1 - FAy3</t>
-  </si>
-  <si>
-    <t>FAz1 - FAz3</t>
-  </si>
-  <si>
-    <t>FBz1 - FBz3</t>
-  </si>
-  <si>
-    <t>FRA1 - FRA3</t>
-  </si>
-  <si>
-    <t>FRB1 - FRB3</t>
-  </si>
-  <si>
-    <t>Resultierende Lagerkraft im Lager A Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>Resultierende Lagerkraft im Lager B Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>FAx1 - FAx3</t>
-  </si>
-  <si>
-    <t>Radiale Lagerkraft B XY-Ebene Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>Radiale Lagerkraft A XY-Ebene Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>Radiale Lagerkraft A XZ-Ebene Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>Radiale Lagerkraft B XZ-Ebene Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>Axiale Lagerkraft A XY/XZ-Ebene Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>Axiale Lagerkraft B XY/XZ-Ebene Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>FBx1 - FBx3</t>
-  </si>
-  <si>
-    <t>s1min - s7min</t>
-  </si>
-  <si>
-    <t>Minimale Länge Strecke s1 bis s7</t>
-  </si>
-  <si>
-    <t>Maximale Länge Strecke s1 bis s7</t>
-  </si>
-  <si>
-    <t>s1max - s7max</t>
-  </si>
-  <si>
-    <t>FN</t>
-  </si>
-  <si>
-    <t>FQ</t>
-  </si>
-  <si>
-    <t>Normalkraft</t>
-  </si>
-  <si>
-    <t>Querkraft</t>
-  </si>
-  <si>
-    <t>Ms1xy - Ms7xy</t>
-  </si>
-  <si>
-    <t>Moment um s1 bis s7 in XY-Ebene</t>
-  </si>
-  <si>
-    <t>Ms1xymin - Ms7xymin</t>
-  </si>
-  <si>
-    <t>Minimales Moment um s1 bis s7 in XY-Ebene</t>
-  </si>
-  <si>
-    <t>Ms1xymax - Ms7xymax</t>
-  </si>
-  <si>
-    <t>Maximales Moment um s1 bis s7 in XY-Ebene</t>
-  </si>
-  <si>
-    <t>s1 - s7</t>
-  </si>
-  <si>
-    <t>Strecken s1 bis s7 für Schnittgrößenverläufe</t>
-  </si>
-  <si>
-    <t>Ms1xz - Ms7xz</t>
-  </si>
-  <si>
-    <t>Moment um s1 bis s7 in XZ-Ebene</t>
-  </si>
-  <si>
-    <t>Ms1xzmax - Ms7xzmax</t>
-  </si>
-  <si>
-    <t>Ms1xzmin - Ms7xzmin</t>
-  </si>
-  <si>
-    <t>Minimales Moment um s1 bis s7 in XZ-Ebene</t>
-  </si>
-  <si>
-    <t>Maximales Moment um s1 bis s7 in XZ-Ebene</t>
-  </si>
-  <si>
-    <t>MsAmax</t>
-  </si>
-  <si>
-    <t>Maximales Drehmoment Antriebswelle</t>
-  </si>
-  <si>
-    <t>Maximales Drehmoment Abtriebswelle</t>
-  </si>
-  <si>
-    <t>Maximales Drehmoment Vorgelegewelle</t>
-  </si>
-  <si>
-    <t>MsVmax</t>
-  </si>
-  <si>
-    <t>MsWmax</t>
-  </si>
-  <si>
-    <t>Biegespannung</t>
-  </si>
-  <si>
-    <t>Torsionsspannung</t>
-  </si>
-  <si>
-    <t>WB1 - WB3</t>
-  </si>
-  <si>
-    <t>WT1 - WB3</t>
-  </si>
-  <si>
-    <t>Biegewiderstandsmoment Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>Torsionswiderstandsmoment Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>σbmax1 - σbmax3</t>
-  </si>
-  <si>
-    <t>τtmax1 - τtmax3</t>
-  </si>
-  <si>
-    <t>Kt1 - Kt3</t>
-  </si>
-  <si>
-    <t>Technologischer Größeneinflussfaktor</t>
-  </si>
-  <si>
-    <t>σbF1 - σbF3</t>
-  </si>
-  <si>
-    <t>τtF1 - τtF3</t>
-  </si>
-  <si>
-    <t>SF1 - SF3</t>
-  </si>
-  <si>
-    <t>Sicherheit Fließgrenze Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>SF1min - SF3min</t>
-  </si>
-  <si>
-    <t>Mindestsicherheit Fließgrenze Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>σba1 - σba3</t>
-  </si>
-  <si>
-    <t>Maximale statische Biegespannung Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>Maximale statische Torsionsspannung Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>Statische Bauteilfestigkeit gegen Biegung Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>Statische Bauteilfestigkeit gegen Torsion Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>Dynamische Biegespannung Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>σbm1 - σbm3</t>
-  </si>
-  <si>
-    <t>Vernachlässigter Faktor dynamische Biegespannung</t>
-  </si>
-  <si>
-    <t>τta1 - τta3</t>
-  </si>
-  <si>
-    <t>τtm1 - τtm3</t>
-  </si>
-  <si>
-    <t>Dynamische Torsionsspannung Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>Vernachlässigter Faktor dynamische Torsionsspannung</t>
-  </si>
-  <si>
-    <t>βkb1 - βkb3</t>
-  </si>
-  <si>
-    <t>Kerbwirkungszahl Biegung Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>βkt1 - βkt3</t>
-  </si>
-  <si>
-    <t>Kerbwirkungszahl Torsion Welle 1 bis 3</t>
-  </si>
-  <si>
-    <t>P1L</t>
-  </si>
-  <si>
-    <t>P1F</t>
-  </si>
-  <si>
-    <t>dynamische Lagerbelastung (Loslager - Antriebswelle)</t>
-  </si>
-  <si>
-    <t>dynamische Lagerbelastung (Festlager - Antriebswelle)</t>
-  </si>
-  <si>
-    <t>l10h</t>
-  </si>
-  <si>
-    <t>anzustrebende nominelle Lebensauer</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>Lebensdauerexponent</t>
-  </si>
-  <si>
-    <t>Cerf</t>
-  </si>
-  <si>
-    <t>erförderliche dynamische Tragzahl</t>
+    <r>
+      <t>τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>tGW1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - τ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>tGW4</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1941,16 +3498,17 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
       <sz val="12.65"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2042,7 +3600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2050,6 +3608,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2364,10 +3923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4572409-E229-4D26-A0D4-41F629C29121}">
-  <dimension ref="A1:B112"/>
+  <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,751 +4089,864 @@
     </row>
     <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>72</v>
+      <c r="A21" s="7" t="s">
+        <v>201</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>73</v>
+      <c r="A22" s="7" t="s">
+        <v>196</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>74</v>
+      <c r="A23" s="7" t="s">
+        <v>197</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>23</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>75</v>
+      <c r="A24" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>76</v>
+      <c r="A25" s="7" t="s">
+        <v>202</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>16</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>195</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>26</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>77</v>
+      <c r="A27" s="7" t="s">
+        <v>198</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>27</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
-        <v>78</v>
+      <c r="A28" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
-        <v>79</v>
+      <c r="A29" s="7" t="s">
+        <v>205</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
-        <v>80</v>
+      <c r="A30" s="7" t="s">
+        <v>206</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
-        <v>97</v>
+      <c r="A38" s="7" t="s">
+        <v>233</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>99</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
-        <v>98</v>
+      <c r="A39" s="7" t="s">
+        <v>234</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>100</v>
+        <v>182</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
-        <v>88</v>
+      <c r="A40" s="7" t="s">
+        <v>236</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>40</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
-        <v>89</v>
+      <c r="A41" s="7" t="s">
+        <v>237</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>41</v>
+        <v>185</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>90</v>
+      <c r="A42" s="7" t="s">
+        <v>232</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>36</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
-        <v>91</v>
+      <c r="A43" s="7" t="s">
+        <v>221</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>44</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
-        <v>92</v>
+      <c r="A44" s="7" t="s">
+        <v>235</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>45</v>
+        <v>183</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A49" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A50" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A51" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A52" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A53" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A54" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A55" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A56" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A57" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A70" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A71" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A72" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A73" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A74" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A75" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A77" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A78" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A79" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A84" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A85" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A88" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
+    <row r="90" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B90" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A50" s="5" t="s">
+    <row r="91" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A91" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
+    <row r="92" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
+    <row r="93" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B93" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
+    <row r="94" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
+    <row r="95" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B95" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B96" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A56" s="5" t="s">
+    <row r="97" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A97" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A57" s="5" t="s">
+    <row r="98" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A98" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A99" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A100" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A58" s="5" t="s">
+    <row r="101" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A101" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A59" s="5" t="s">
+    <row r="102" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A102" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B102" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A60" s="5" t="s">
+    <row r="103" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A103" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B103" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A61" s="5" t="s">
+    <row r="104" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A104" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B104" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A62" s="5" t="s">
+    <row r="105" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A105" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B105" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B106" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A64" s="5" t="s">
+    <row r="107" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A107" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A108" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A109" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A110" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A111" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A112" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A113" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A114" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A115" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A116" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A117" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A118" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A119" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B119" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B69" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B70" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B71" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="B72" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="B73" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B74" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B75" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="B76" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="B77" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="B78" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B79" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="B80" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B81" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="B82" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B83" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="B84" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B85" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B86" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B87" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="6" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="6"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="6"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="6"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="6"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B124" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="B88" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B89" t="s">
+      <c r="B125" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="6" t="s">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B126" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="6" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B127" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="B91" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
+      <c r="B128" t="s">
         <v>180</v>
       </c>
-      <c r="B92" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B93" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="B94" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="B95" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="B96" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="B97" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="B98" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="B99" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="B100" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="B101" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="B102" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="B103" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="B104" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="B105" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="B106" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="B107" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="B108" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="B109" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="B110" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="B111" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="B112" t="s">
-        <v>222</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;CMaschinenelemente Entwurf 3
+Jade Hochschule Wilhelmshaven</oddHeader>
+    <oddFooter>&amp;LDaniel Skrypnikov&amp;CEdis Duvnjak&amp;RMarvin Müller</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>